<commit_message>
Feat/client review visit types (#828)
* fix: change PAE icon

* feat: specifying physical client review
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC02BB-13B5-CC47-8747-E8A0F52E2519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B7AA34-C0E3-B94F-A7C2-AB4E26A7C81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="234">
   <si>
     <t>type</t>
   </si>
@@ -393,13 +393,6 @@
   </si>
   <si>
     <t>tracing_methods</t>
-  </si>
-  <si>
-    <t>in_person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Yes, Via Physical visit
-</t>
   </si>
   <si>
     <t xml:space="preserve">2. Yes, Via Phone call
@@ -725,6 +718,20 @@
   </si>
   <si>
     <t>health_center</t>
+  </si>
+  <si>
+    <t>in_person_home</t>
+  </si>
+  <si>
+    <t>in_person_clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Yes, Via physical home visit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Yes, Via physical clinic visit
+</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1760,7 +1767,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>52</v>
@@ -1791,7 +1798,7 @@
     </row>
     <row r="22" spans="1:26" ht="16">
       <c r="A22" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>30</v>
@@ -3588,18 +3595,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
@@ -3712,566 +3719,576 @@
         <v>121</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="12" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="C16" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>144</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>158</v>
+      <c r="A24" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="16">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16">
       <c r="A30" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16">
       <c r="A31" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A37" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C38" s="33" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
-      <c r="S37" s="33"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="33"/>
-      <c r="V37" s="33"/>
-      <c r="W37" s="33"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
-      <c r="Z37" s="33"/>
-    </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>186</v>
-      </c>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33"/>
+      <c r="S38" s="33"/>
+      <c r="T38" s="33"/>
+      <c r="U38" s="33"/>
+      <c r="V38" s="33"/>
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+      <c r="Y38" s="33"/>
+      <c r="Z38" s="33"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D40" s="34"/>
+      <c r="A40" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D41" s="34"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D42" s="34"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D43" s="34"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D44" s="34"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D45" s="34"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D46" s="34"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D47" s="34"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D48" s="34"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D49" s="34"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D50" s="34"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D51" s="34"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D52" s="34"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D53" s="34"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D54" s="34"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D55" s="34"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D56" s="34"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D57" s="34"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D58" s="34"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D59" s="34"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" s="33" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1"/>
+      <c r="A60" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D60" s="34"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A61" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>227</v>
+      </c>
+    </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
@@ -5203,6 +5220,7 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5227,31 +5245,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>132</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>134</v>
       </c>
       <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
@@ -5273,29 +5291,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="32">
         <v>43894</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>

</xml_diff>

<commit_message>
Aurum stepwegde/day 3 task (#1053)
* feat: day 3 task

* feat: show minor attributes on contact profile

* feat: add priority to minor no contact

* fix: edit person for minor

* fix: clear related tasks

* feat: clean referal translation
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B7AA34-C0E3-B94F-A7C2-AB4E26A7C81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331DC98-A299-0048-84F0-C30C612473CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
   <si>
     <t>type</t>
   </si>
@@ -98,18 +98,6 @@
     <t>Source ID</t>
   </si>
   <si>
-    <t>is_referral_for_care_ctx</t>
-  </si>
-  <si>
-    <t>Is a referral for care case</t>
-  </si>
-  <si>
-    <t>is_no_contact_ctx</t>
-  </si>
-  <si>
-    <t>Is a no contact case</t>
-  </si>
-  <si>
     <t>contact</t>
   </si>
   <si>
@@ -170,18 +158,6 @@
     <t>../inputs/contact/phone</t>
   </si>
   <si>
-    <t>is_referral_for_care</t>
-  </si>
-  <si>
-    <t>../inputs/is_referral_for_care</t>
-  </si>
-  <si>
-    <t>is_no_contact</t>
-  </si>
-  <si>
-    <t>../inputs/is_no_contact</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -194,9 +170,6 @@
     <t>client_came</t>
   </si>
   <si>
-    <t>Did client return to clinic?</t>
-  </si>
-  <si>
     <t>return_client</t>
   </si>
   <si>
@@ -227,42 +200,6 @@
     <t>Date is not in the future: and not more than 4 weeks ago</t>
   </si>
   <si>
-    <t>ae_positive</t>
-  </si>
-  <si>
-    <t>Did nurse identify an AE?</t>
-  </si>
-  <si>
-    <t>select_one severities</t>
-  </si>
-  <si>
-    <t>ae_severity</t>
-  </si>
-  <si>
-    <t>Severity of the Adverse Event (AE)</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes'</t>
-  </si>
-  <si>
-    <t>ae_type</t>
-  </si>
-  <si>
-    <t>AE Code</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\-]+$")</t>
-  </si>
-  <si>
-    <t>The AE Code should be captured in the same way they are recorded in the VMMC register</t>
-  </si>
-  <si>
-    <t>Should be the same AE Code as the one used in the register</t>
-  </si>
-  <si>
-    <t>trace_client</t>
-  </si>
-  <si>
     <t>${client_came}='no'</t>
   </si>
   <si>
@@ -275,66 +212,9 @@
     <t>Have you traced the client?</t>
   </si>
   <si>
-    <t>client_traced</t>
-  </si>
-  <si>
-    <t>if(${tracing_method} = 'in_person', 'yes', if(${tracing_method} = 'phone', 'yes', 'no'))</t>
-  </si>
-  <si>
-    <t>client_not_traced_reason</t>
-  </si>
-  <si>
-    <t>If no tracing, explain why not.</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'no'</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'yes'</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>n_thanks</t>
-  </si>
-  <si>
-    <t>Thanks for tracing the client</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'yes'</t>
-  </si>
-  <si>
-    <t>q_ae_positive</t>
-  </si>
-  <si>
-    <t>if(${tracing_method} = "in_person", "Did nurse identify an AE?", "Did nurse suspect an AE?")</t>
-  </si>
-  <si>
-    <t>${q_ae_positive}</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'no'</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes' and ${tracing_method} = 'in_person'</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>additional_comments</t>
-  </si>
-  <si>
-    <t>Any Additional Comments</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -395,22 +275,6 @@
     <t>tracing_methods</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Yes, Via Phone call
-</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>3. No</t>
-  </si>
-  <si>
-    <t>facilities</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -453,285 +317,82 @@
     <t>en</t>
   </si>
   <si>
-    <t>guruve_hospital</t>
-  </si>
-  <si>
-    <t>1. Guruve Hospital</t>
-  </si>
-  <si>
-    <t>bepura_clinic</t>
-  </si>
-  <si>
-    <t>2. Bepura Clinic</t>
-  </si>
-  <si>
-    <t>mhondoro_ngezi</t>
-  </si>
-  <si>
-    <t>3. Mhondoro Ngezi</t>
-  </si>
-  <si>
-    <t>michael_hospital</t>
-  </si>
-  <si>
-    <t>4. St Michael’s Hospital</t>
-  </si>
-  <si>
-    <t>turf_clinic</t>
-  </si>
-  <si>
-    <t>5. Turf Clinic</t>
-  </si>
-  <si>
-    <t>donain_clinic</t>
-  </si>
-  <si>
-    <t>6. Donain Clinic</t>
-  </si>
-  <si>
-    <t>matobo_district</t>
-  </si>
-  <si>
-    <t>7. Matobo District</t>
-  </si>
-  <si>
-    <t>maphisa_hospital</t>
-  </si>
-  <si>
-    <t>8. Maphisa Hospital</t>
-  </si>
-  <si>
-    <t>tshelanyemba_hospital</t>
-  </si>
-  <si>
-    <t>9. Tshelanyemba Hospital</t>
-  </si>
-  <si>
-    <t>joseph_hospital</t>
-  </si>
-  <si>
-    <t>10. St Joseph Hospital</t>
-  </si>
-  <si>
-    <t>matobo_rural_hospital</t>
-  </si>
-  <si>
-    <t>11. Matobo Rural Hospital</t>
-  </si>
-  <si>
-    <t>sanyati_baptist_hospital</t>
-  </si>
-  <si>
-    <t>12. Sanyati Baptist Hospital</t>
-  </si>
-  <si>
-    <t>chakari_clinic</t>
-  </si>
-  <si>
-    <t>13. Chakari Clinic</t>
-  </si>
-  <si>
-    <t>gokwe_district_hospital</t>
-  </si>
-  <si>
-    <t>14. Gokwe District Hospital</t>
-  </si>
-  <si>
-    <t>sai_clinic</t>
-  </si>
-  <si>
-    <t>15. Sai Clinic</t>
-  </si>
-  <si>
-    <t>kana_mission_hospital</t>
-  </si>
-  <si>
-    <t>16. Kana Mission Hospital</t>
-  </si>
-  <si>
-    <t>chidamoyo_mission_hospital</t>
-  </si>
-  <si>
-    <t>17. Chidamoyo Mission Hospital</t>
-  </si>
-  <si>
-    <t>hurungwe_rural_hospital</t>
-  </si>
-  <si>
-    <t>18. Hurungwe Rural Hospital</t>
-  </si>
-  <si>
-    <t>karoi_district_hospital</t>
-  </si>
-  <si>
-    <t>19. Karoi District Hospital</t>
-  </si>
-  <si>
-    <t>chitsungo_mission_hospital</t>
-  </si>
-  <si>
-    <t>20. Chitsungo Mission Hospital</t>
-  </si>
-  <si>
-    <t>mahuwe_rhc</t>
-  </si>
-  <si>
-    <t>21. Mahuwe RHC</t>
-  </si>
-  <si>
-    <t>luke_mission_hospital</t>
-  </si>
-  <si>
-    <t>22. St Luke's Mission Hospital</t>
-  </si>
-  <si>
-    <t>Paul_mission_hospital</t>
-  </si>
-  <si>
-    <t>23. Paul's Mission Hospital</t>
-  </si>
-  <si>
-    <t>seke_north</t>
-  </si>
-  <si>
-    <t>seke_south</t>
-  </si>
-  <si>
-    <t>city_med</t>
-  </si>
-  <si>
-    <t>zengeza</t>
-  </si>
-  <si>
-    <t>chitungwiza_central</t>
-  </si>
-  <si>
-    <t>chegutu_norton</t>
-  </si>
-  <si>
-    <t>chegutu_district</t>
-  </si>
-  <si>
-    <t>monera</t>
-  </si>
-  <si>
-    <t>marondera</t>
-  </si>
-  <si>
-    <t>mahusekwa</t>
-  </si>
-  <si>
-    <t>makumbe</t>
-  </si>
-  <si>
-    <t>ruwa</t>
-  </si>
-  <si>
-    <t>kadoma</t>
-  </si>
-  <si>
-    <t>kadoma_city</t>
-  </si>
-  <si>
-    <t>ndanga</t>
-  </si>
-  <si>
-    <t>musiso</t>
-  </si>
-  <si>
-    <t>mnene</t>
-  </si>
-  <si>
-    <t>musume</t>
-  </si>
-  <si>
-    <t>mberengwa</t>
-  </si>
-  <si>
-    <t>masase</t>
-  </si>
-  <si>
-    <t>24. Chitungwiza-Seke North clinic</t>
-  </si>
-  <si>
-    <t>25. Chitungwiza-Seke South clinic</t>
-  </si>
-  <si>
-    <t>26. Chitungwiza-City Med hospital</t>
-  </si>
-  <si>
-    <t>27. Chitungwiza-Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>28. Chitungwiza-Chitungwiza Central Hospital</t>
-  </si>
-  <si>
-    <t>29. Chegutu- Norton hospital</t>
-  </si>
-  <si>
-    <t>30. Chegutu- District Hospital</t>
-  </si>
-  <si>
-    <t>31. Chegutu-Monera clinic(Norton Outreach)</t>
-  </si>
-  <si>
-    <t>32. Marondera- Marondera District Hospital</t>
-  </si>
-  <si>
-    <t>33. Marondera- Mahusekwa Hospital</t>
-  </si>
-  <si>
-    <t>34. Goromonzi-Makumbe Mission Hospital</t>
-  </si>
-  <si>
-    <t>35. Goromonzi-Ruwa Rehab Hospital</t>
-  </si>
-  <si>
-    <t>36. Sanyati-Kadoma Hospital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37. Sanyati-Kadoma City </t>
-  </si>
-  <si>
-    <t>38. Zaka-Ndanga District Hospital</t>
-  </si>
-  <si>
-    <t>39. Zaka-Musiso Mission Hospital</t>
-  </si>
-  <si>
-    <t>40. Mberengwa-Mnene Mission Hospital</t>
-  </si>
-  <si>
-    <t>41. Mberengwa-Musume Mission Hospital</t>
-  </si>
-  <si>
-    <t>42. Mberengwa-Mberengwa District Hospital</t>
-  </si>
-  <si>
-    <t>43. Mberengwa-Masase Mission Hospital</t>
-  </si>
-  <si>
-    <t>44. Other</t>
-  </si>
-  <si>
     <t>db:health_center</t>
   </si>
   <si>
     <t>health_center</t>
   </si>
   <si>
-    <t>in_person_home</t>
-  </si>
-  <si>
-    <t>in_person_clinic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Yes, Via physical home visit
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Yes, Via physical clinic visit
-</t>
+    <t>Was client seen by a clinician?</t>
+  </si>
+  <si>
+    <t>client_visit</t>
+  </si>
+  <si>
+    <t>chaps_mc_clinic</t>
+  </si>
+  <si>
+    <t>doh</t>
+  </si>
+  <si>
+    <t>DOH</t>
+  </si>
+  <si>
+    <t>private_clinic</t>
+  </si>
+  <si>
+    <t>CHAPS MC team</t>
+  </si>
+  <si>
+    <t>Private clinic</t>
+  </si>
+  <si>
+    <t>select_one client_visit</t>
+  </si>
+  <si>
+    <t>Which facility?</t>
+  </si>
+  <si>
+    <t>selected(${client_visit}, 'chaps_mc_clinic')</t>
+  </si>
+  <si>
+    <t>client_visit_location</t>
+  </si>
+  <si>
+    <t>Specify</t>
+  </si>
+  <si>
+    <t>selected(${client_visit}, 'doh') or selected(${client_visit}, 'private_clinic')</t>
+  </si>
+  <si>
+    <t>Client reached by phone and is ok</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>Client responded via SMS and is ok</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>explain</t>
+  </si>
+  <si>
+    <t>Please Explain</t>
+  </si>
+  <si>
+    <t>selected(${tracing_method}, 'unknown')</t>
+  </si>
+  <si>
+    <t>No (Creates TRACE CLIENT task)</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
   </si>
 </sst>
 </file>
@@ -741,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -795,16 +456,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Cambria"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -836,8 +487,26 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,12 +517,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2E75B6"/>
         <bgColor rgb="FF2E75B6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -891,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -934,38 +597,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,11 +837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1198,7 +854,10 @@
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="26" width="11.5" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="13" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16">
@@ -1235,7 +894,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="34" t="s">
+        <v>121</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1319,19 +980,17 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="16">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1340,38 +999,44 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="16">
-      <c r="A6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="16">
       <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1381,43 +1046,33 @@
     </row>
     <row r="8" spans="1:26" ht="16">
       <c r="A8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="E8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="16">
       <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1426,19 +1081,13 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1447,44 +1096,90 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="16">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
     </row>
     <row r="12" spans="1:26" ht="16">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
     </row>
     <row r="13" spans="1:26" ht="16">
-      <c r="A13" s="13" t="s">
-        <v>39</v>
+      <c r="A13" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1494,180 +1189,180 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="C15" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="16">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
+      <c r="C16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" ht="16">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="A17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" ht="16">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1691,26 +1386,30 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="16">
-      <c r="A19" s="8" t="s">
-        <v>53</v>
+      <c r="A19" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="L19" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -1727,22 +1426,20 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="16">
-      <c r="A20" s="13" t="s">
-        <v>11</v>
+      <c r="A20" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1764,14 +1461,10 @@
     </row>
     <row r="21" spans="1:26" ht="16">
       <c r="A21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>52</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1797,24 +1490,22 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="16">
-      <c r="A22" s="12" t="s">
-        <v>228</v>
+      <c r="A22" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+        <v>109</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1835,20 +1526,26 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="16">
-      <c r="A23" s="12" t="s">
-        <v>16</v>
+      <c r="A23" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1870,10 +1567,10 @@
     </row>
     <row r="24" spans="1:26" ht="16">
       <c r="A24" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1899,26 +1596,24 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="16">
-      <c r="A25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="8"/>
+      <c r="A25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="F25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1938,20 +1633,22 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="16">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -1974,25 +1671,27 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="16">
-      <c r="A27" s="8" t="s">
-        <v>68</v>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A27" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -2012,611 +1711,41 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" spans="1:26" ht="16">
-      <c r="A28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-    </row>
-    <row r="29" spans="1:26" ht="16">
-      <c r="A29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-    </row>
-    <row r="30" spans="1:26" ht="16">
-      <c r="A30" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-    </row>
-    <row r="31" spans="1:26" ht="16">
-      <c r="A31" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-    </row>
-    <row r="32" spans="1:26" ht="16">
-      <c r="A32" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-    </row>
-    <row r="33" spans="1:26" ht="16">
-      <c r="A33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-    </row>
-    <row r="35" spans="1:26" ht="16">
-      <c r="A35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-    </row>
-    <row r="36" spans="1:26" ht="16">
-      <c r="A36" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-    </row>
-    <row r="37" spans="1:26" ht="16">
-      <c r="A37" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-    </row>
-    <row r="38" spans="1:26" ht="16">
-      <c r="A38" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-    </row>
-    <row r="39" spans="1:26" ht="16">
-      <c r="A39" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-    </row>
-    <row r="40" spans="1:26" ht="16">
-      <c r="A40" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-    </row>
-    <row r="41" spans="1:26" ht="16">
-      <c r="A41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-    </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="8"/>
-    </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="8"/>
-      <c r="X43" s="8"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="8"/>
-    </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3571,22 +2700,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
-    <row r="1010" ht="15.75" customHeight="1"/>
-    <row r="1011" ht="15.75" customHeight="1"/>
-    <row r="1012" ht="15.75" customHeight="1"/>
-    <row r="1013" ht="15.75" customHeight="1"/>
-    <row r="1014" ht="15.75" customHeight="1"/>
-    <row r="1015" ht="15.75" customHeight="1"/>
-    <row r="1016" ht="15.75" customHeight="1"/>
-    <row r="1017" ht="15.75" customHeight="1"/>
-    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -3597,15 +2710,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
@@ -3613,7 +2726,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3624,30 +2737,30 @@
     </row>
     <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="27"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1"/>
@@ -3656,35 +2769,35 @@
     </row>
     <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -3694,68 +2807,68 @@
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>230</v>
+        <v>32</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>231</v>
+        <v>113</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>233</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>122</v>
+        <v>62</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
@@ -3764,530 +2877,284 @@
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>142</v>
+      <c r="A18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>144</v>
+      <c r="A19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>146</v>
+      <c r="A20" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>148</v>
-      </c>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>150</v>
-      </c>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>152</v>
-      </c>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>154</v>
-      </c>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>156</v>
-      </c>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>158</v>
-      </c>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>160</v>
-      </c>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>162</v>
-      </c>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>164</v>
-      </c>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3" ht="16">
-      <c r="A30" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>166</v>
-      </c>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3" ht="16">
-      <c r="A31" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>168</v>
-      </c>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>170</v>
-      </c>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>172</v>
-      </c>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>174</v>
-      </c>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>176</v>
-      </c>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>178</v>
-      </c>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33"/>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+    </row>
+    <row r="38" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="33" t="s">
-        <v>186</v>
-      </c>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D41" s="34"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" s="34"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D43" s="34"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D44" s="34"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D45" s="34"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D46" s="34"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D47" s="34"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D48" s="34"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D49" s="34"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="30"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A50" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D50" s="34"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A51" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D51" s="34"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="30"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A52" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D52" s="34"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A53" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D53" s="34"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="30"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A54" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D54" s="34"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A55" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D55" s="34"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="30"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A56" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D56" s="34"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A57" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D57" s="34"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="30"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" s="34"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D59" s="34"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="30"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D60" s="34"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="30"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A61" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="B61" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" s="33" t="s">
-        <v>227</v>
-      </c>
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
@@ -5244,94 +4111,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" s="28" t="s">
+      <c r="A1" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="H1" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="32">
+      <c r="A2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="28">
         <v>43894</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
+      <c r="D2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Minor day 3 task and improved client review and referral tasks
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC02BB-13B5-CC47-8747-E8A0F52E2519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331DC98-A299-0048-84F0-C30C612473CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
   <si>
     <t>type</t>
   </si>
@@ -98,18 +98,6 @@
     <t>Source ID</t>
   </si>
   <si>
-    <t>is_referral_for_care_ctx</t>
-  </si>
-  <si>
-    <t>Is a referral for care case</t>
-  </si>
-  <si>
-    <t>is_no_contact_ctx</t>
-  </si>
-  <si>
-    <t>Is a no contact case</t>
-  </si>
-  <si>
     <t>contact</t>
   </si>
   <si>
@@ -170,18 +158,6 @@
     <t>../inputs/contact/phone</t>
   </si>
   <si>
-    <t>is_referral_for_care</t>
-  </si>
-  <si>
-    <t>../inputs/is_referral_for_care</t>
-  </si>
-  <si>
-    <t>is_no_contact</t>
-  </si>
-  <si>
-    <t>../inputs/is_no_contact</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -194,9 +170,6 @@
     <t>client_came</t>
   </si>
   <si>
-    <t>Did client return to clinic?</t>
-  </si>
-  <si>
     <t>return_client</t>
   </si>
   <si>
@@ -227,42 +200,6 @@
     <t>Date is not in the future: and not more than 4 weeks ago</t>
   </si>
   <si>
-    <t>ae_positive</t>
-  </si>
-  <si>
-    <t>Did nurse identify an AE?</t>
-  </si>
-  <si>
-    <t>select_one severities</t>
-  </si>
-  <si>
-    <t>ae_severity</t>
-  </si>
-  <si>
-    <t>Severity of the Adverse Event (AE)</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes'</t>
-  </si>
-  <si>
-    <t>ae_type</t>
-  </si>
-  <si>
-    <t>AE Code</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\-]+$")</t>
-  </si>
-  <si>
-    <t>The AE Code should be captured in the same way they are recorded in the VMMC register</t>
-  </si>
-  <si>
-    <t>Should be the same AE Code as the one used in the register</t>
-  </si>
-  <si>
-    <t>trace_client</t>
-  </si>
-  <si>
     <t>${client_came}='no'</t>
   </si>
   <si>
@@ -275,66 +212,9 @@
     <t>Have you traced the client?</t>
   </si>
   <si>
-    <t>client_traced</t>
-  </si>
-  <si>
-    <t>if(${tracing_method} = 'in_person', 'yes', if(${tracing_method} = 'phone', 'yes', 'no'))</t>
-  </si>
-  <si>
-    <t>client_not_traced_reason</t>
-  </si>
-  <si>
-    <t>If no tracing, explain why not.</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'no'</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'yes'</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>n_thanks</t>
-  </si>
-  <si>
-    <t>Thanks for tracing the client</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'yes'</t>
-  </si>
-  <si>
-    <t>q_ae_positive</t>
-  </si>
-  <si>
-    <t>if(${tracing_method} = "in_person", "Did nurse identify an AE?", "Did nurse suspect an AE?")</t>
-  </si>
-  <si>
-    <t>${q_ae_positive}</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'no'</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes' and ${tracing_method} = 'in_person'</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>additional_comments</t>
-  </si>
-  <si>
-    <t>Any Additional Comments</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -395,29 +275,6 @@
     <t>tracing_methods</t>
   </si>
   <si>
-    <t>in_person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Yes, Via Physical visit
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Yes, Via Phone call
-</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>3. No</t>
-  </si>
-  <si>
-    <t>facilities</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -460,271 +317,82 @@
     <t>en</t>
   </si>
   <si>
-    <t>guruve_hospital</t>
-  </si>
-  <si>
-    <t>1. Guruve Hospital</t>
-  </si>
-  <si>
-    <t>bepura_clinic</t>
-  </si>
-  <si>
-    <t>2. Bepura Clinic</t>
-  </si>
-  <si>
-    <t>mhondoro_ngezi</t>
-  </si>
-  <si>
-    <t>3. Mhondoro Ngezi</t>
-  </si>
-  <si>
-    <t>michael_hospital</t>
-  </si>
-  <si>
-    <t>4. St Michael’s Hospital</t>
-  </si>
-  <si>
-    <t>turf_clinic</t>
-  </si>
-  <si>
-    <t>5. Turf Clinic</t>
-  </si>
-  <si>
-    <t>donain_clinic</t>
-  </si>
-  <si>
-    <t>6. Donain Clinic</t>
-  </si>
-  <si>
-    <t>matobo_district</t>
-  </si>
-  <si>
-    <t>7. Matobo District</t>
-  </si>
-  <si>
-    <t>maphisa_hospital</t>
-  </si>
-  <si>
-    <t>8. Maphisa Hospital</t>
-  </si>
-  <si>
-    <t>tshelanyemba_hospital</t>
-  </si>
-  <si>
-    <t>9. Tshelanyemba Hospital</t>
-  </si>
-  <si>
-    <t>joseph_hospital</t>
-  </si>
-  <si>
-    <t>10. St Joseph Hospital</t>
-  </si>
-  <si>
-    <t>matobo_rural_hospital</t>
-  </si>
-  <si>
-    <t>11. Matobo Rural Hospital</t>
-  </si>
-  <si>
-    <t>sanyati_baptist_hospital</t>
-  </si>
-  <si>
-    <t>12. Sanyati Baptist Hospital</t>
-  </si>
-  <si>
-    <t>chakari_clinic</t>
-  </si>
-  <si>
-    <t>13. Chakari Clinic</t>
-  </si>
-  <si>
-    <t>gokwe_district_hospital</t>
-  </si>
-  <si>
-    <t>14. Gokwe District Hospital</t>
-  </si>
-  <si>
-    <t>sai_clinic</t>
-  </si>
-  <si>
-    <t>15. Sai Clinic</t>
-  </si>
-  <si>
-    <t>kana_mission_hospital</t>
-  </si>
-  <si>
-    <t>16. Kana Mission Hospital</t>
-  </si>
-  <si>
-    <t>chidamoyo_mission_hospital</t>
-  </si>
-  <si>
-    <t>17. Chidamoyo Mission Hospital</t>
-  </si>
-  <si>
-    <t>hurungwe_rural_hospital</t>
-  </si>
-  <si>
-    <t>18. Hurungwe Rural Hospital</t>
-  </si>
-  <si>
-    <t>karoi_district_hospital</t>
-  </si>
-  <si>
-    <t>19. Karoi District Hospital</t>
-  </si>
-  <si>
-    <t>chitsungo_mission_hospital</t>
-  </si>
-  <si>
-    <t>20. Chitsungo Mission Hospital</t>
-  </si>
-  <si>
-    <t>mahuwe_rhc</t>
-  </si>
-  <si>
-    <t>21. Mahuwe RHC</t>
-  </si>
-  <si>
-    <t>luke_mission_hospital</t>
-  </si>
-  <si>
-    <t>22. St Luke's Mission Hospital</t>
-  </si>
-  <si>
-    <t>Paul_mission_hospital</t>
-  </si>
-  <si>
-    <t>23. Paul's Mission Hospital</t>
-  </si>
-  <si>
-    <t>seke_north</t>
-  </si>
-  <si>
-    <t>seke_south</t>
-  </si>
-  <si>
-    <t>city_med</t>
-  </si>
-  <si>
-    <t>zengeza</t>
-  </si>
-  <si>
-    <t>chitungwiza_central</t>
-  </si>
-  <si>
-    <t>chegutu_norton</t>
-  </si>
-  <si>
-    <t>chegutu_district</t>
-  </si>
-  <si>
-    <t>monera</t>
-  </si>
-  <si>
-    <t>marondera</t>
-  </si>
-  <si>
-    <t>mahusekwa</t>
-  </si>
-  <si>
-    <t>makumbe</t>
-  </si>
-  <si>
-    <t>ruwa</t>
-  </si>
-  <si>
-    <t>kadoma</t>
-  </si>
-  <si>
-    <t>kadoma_city</t>
-  </si>
-  <si>
-    <t>ndanga</t>
-  </si>
-  <si>
-    <t>musiso</t>
-  </si>
-  <si>
-    <t>mnene</t>
-  </si>
-  <si>
-    <t>musume</t>
-  </si>
-  <si>
-    <t>mberengwa</t>
-  </si>
-  <si>
-    <t>masase</t>
-  </si>
-  <si>
-    <t>24. Chitungwiza-Seke North clinic</t>
-  </si>
-  <si>
-    <t>25. Chitungwiza-Seke South clinic</t>
-  </si>
-  <si>
-    <t>26. Chitungwiza-City Med hospital</t>
-  </si>
-  <si>
-    <t>27. Chitungwiza-Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>28. Chitungwiza-Chitungwiza Central Hospital</t>
-  </si>
-  <si>
-    <t>29. Chegutu- Norton hospital</t>
-  </si>
-  <si>
-    <t>30. Chegutu- District Hospital</t>
-  </si>
-  <si>
-    <t>31. Chegutu-Monera clinic(Norton Outreach)</t>
-  </si>
-  <si>
-    <t>32. Marondera- Marondera District Hospital</t>
-  </si>
-  <si>
-    <t>33. Marondera- Mahusekwa Hospital</t>
-  </si>
-  <si>
-    <t>34. Goromonzi-Makumbe Mission Hospital</t>
-  </si>
-  <si>
-    <t>35. Goromonzi-Ruwa Rehab Hospital</t>
-  </si>
-  <si>
-    <t>36. Sanyati-Kadoma Hospital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37. Sanyati-Kadoma City </t>
-  </si>
-  <si>
-    <t>38. Zaka-Ndanga District Hospital</t>
-  </si>
-  <si>
-    <t>39. Zaka-Musiso Mission Hospital</t>
-  </si>
-  <si>
-    <t>40. Mberengwa-Mnene Mission Hospital</t>
-  </si>
-  <si>
-    <t>41. Mberengwa-Musume Mission Hospital</t>
-  </si>
-  <si>
-    <t>42. Mberengwa-Mberengwa District Hospital</t>
-  </si>
-  <si>
-    <t>43. Mberengwa-Masase Mission Hospital</t>
-  </si>
-  <si>
-    <t>44. Other</t>
-  </si>
-  <si>
     <t>db:health_center</t>
   </si>
   <si>
     <t>health_center</t>
+  </si>
+  <si>
+    <t>Was client seen by a clinician?</t>
+  </si>
+  <si>
+    <t>client_visit</t>
+  </si>
+  <si>
+    <t>chaps_mc_clinic</t>
+  </si>
+  <si>
+    <t>doh</t>
+  </si>
+  <si>
+    <t>DOH</t>
+  </si>
+  <si>
+    <t>private_clinic</t>
+  </si>
+  <si>
+    <t>CHAPS MC team</t>
+  </si>
+  <si>
+    <t>Private clinic</t>
+  </si>
+  <si>
+    <t>select_one client_visit</t>
+  </si>
+  <si>
+    <t>Which facility?</t>
+  </si>
+  <si>
+    <t>selected(${client_visit}, 'chaps_mc_clinic')</t>
+  </si>
+  <si>
+    <t>client_visit_location</t>
+  </si>
+  <si>
+    <t>Specify</t>
+  </si>
+  <si>
+    <t>selected(${client_visit}, 'doh') or selected(${client_visit}, 'private_clinic')</t>
+  </si>
+  <si>
+    <t>Client reached by phone and is ok</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>Client responded via SMS and is ok</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>explain</t>
+  </si>
+  <si>
+    <t>Please Explain</t>
+  </si>
+  <si>
+    <t>selected(${tracing_method}, 'unknown')</t>
+  </si>
+  <si>
+    <t>No (Creates TRACE CLIENT task)</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
   </si>
 </sst>
 </file>
@@ -734,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -788,16 +456,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Cambria"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -829,8 +487,26 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,12 +517,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2E75B6"/>
         <bgColor rgb="FF2E75B6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -884,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -927,38 +597,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,11 +837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1191,7 +854,10 @@
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="26" width="11.5" customWidth="1"/>
+    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="13" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16">
@@ -1228,7 +894,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="34" t="s">
+        <v>121</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1312,19 +980,17 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="16">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1333,38 +999,44 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="16">
-      <c r="A6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="16">
       <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1374,43 +1046,33 @@
     </row>
     <row r="8" spans="1:26" ht="16">
       <c r="A8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="E8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="16">
       <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1419,19 +1081,13 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1440,44 +1096,90 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="16">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
     </row>
     <row r="12" spans="1:26" ht="16">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
     </row>
     <row r="13" spans="1:26" ht="16">
-      <c r="A13" s="13" t="s">
-        <v>39</v>
+      <c r="A13" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1487,180 +1189,180 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
+        <v>42</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="15" t="s">
+      <c r="C14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="C15" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="16">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1" t="s">
+      <c r="C16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" ht="16">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="A17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26" ht="16">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
-        <v>15</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1684,26 +1386,30 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="16">
-      <c r="A19" s="8" t="s">
-        <v>53</v>
+      <c r="A19" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="L19" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -1720,22 +1426,20 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="16">
-      <c r="A20" s="13" t="s">
-        <v>11</v>
+      <c r="A20" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1757,14 +1461,10 @@
     </row>
     <row r="21" spans="1:26" ht="16">
       <c r="A21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>52</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1790,24 +1490,22 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="16">
-      <c r="A22" s="12" t="s">
-        <v>230</v>
+      <c r="A22" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+        <v>109</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1828,20 +1526,26 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="16">
-      <c r="A23" s="12" t="s">
-        <v>16</v>
+      <c r="A23" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1863,10 +1567,10 @@
     </row>
     <row r="24" spans="1:26" ht="16">
       <c r="A24" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -1892,26 +1596,24 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="16">
-      <c r="A25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="8"/>
+      <c r="A25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="F25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1931,20 +1633,22 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="16">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -1967,25 +1671,27 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="16">
-      <c r="A27" s="8" t="s">
-        <v>68</v>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A27" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -2005,611 +1711,41 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" spans="1:26" ht="16">
-      <c r="A28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-    </row>
-    <row r="29" spans="1:26" ht="16">
-      <c r="A29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-    </row>
-    <row r="30" spans="1:26" ht="16">
-      <c r="A30" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-    </row>
-    <row r="31" spans="1:26" ht="16">
-      <c r="A31" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-    </row>
-    <row r="32" spans="1:26" ht="16">
-      <c r="A32" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-    </row>
-    <row r="33" spans="1:26" ht="16">
-      <c r="A33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-    </row>
-    <row r="35" spans="1:26" ht="16">
-      <c r="A35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-    </row>
-    <row r="36" spans="1:26" ht="16">
-      <c r="A36" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-    </row>
-    <row r="37" spans="1:26" ht="16">
-      <c r="A37" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-    </row>
-    <row r="38" spans="1:26" ht="16">
-      <c r="A38" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-    </row>
-    <row r="39" spans="1:26" ht="16">
-      <c r="A39" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-    </row>
-    <row r="40" spans="1:26" ht="16">
-      <c r="A40" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-    </row>
-    <row r="41" spans="1:26" ht="16">
-      <c r="A41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-    </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="8"/>
-    </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H43" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="8"/>
-      <c r="X43" s="8"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="8"/>
-    </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3564,22 +2700,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
-    <row r="1005" ht="15.75" customHeight="1"/>
-    <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
-    <row r="1010" ht="15.75" customHeight="1"/>
-    <row r="1011" ht="15.75" customHeight="1"/>
-    <row r="1012" ht="15.75" customHeight="1"/>
-    <row r="1013" ht="15.75" customHeight="1"/>
-    <row r="1014" ht="15.75" customHeight="1"/>
-    <row r="1015" ht="15.75" customHeight="1"/>
-    <row r="1016" ht="15.75" customHeight="1"/>
-    <row r="1017" ht="15.75" customHeight="1"/>
-    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -3588,25 +2708,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3617,30 +2737,30 @@
     </row>
     <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="27"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1"/>
@@ -3649,35 +2769,35 @@
     </row>
     <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -3687,591 +2807,355 @@
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>150</v>
+      <c r="A20" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>152</v>
-      </c>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>154</v>
-      </c>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>156</v>
-      </c>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>158</v>
-      </c>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>160</v>
-      </c>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>162</v>
-      </c>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>164</v>
-      </c>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="16">
-      <c r="A29" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>168</v>
-      </c>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3" ht="16">
-      <c r="A30" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>172</v>
-      </c>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+    </row>
+    <row r="31" spans="1:3" ht="16">
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>174</v>
-      </c>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>176</v>
-      </c>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>178</v>
-      </c>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>180</v>
-      </c>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="C37" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
-      <c r="S37" s="33"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="33"/>
-      <c r="V37" s="33"/>
-      <c r="W37" s="33"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
-      <c r="Z37" s="33"/>
-    </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>186</v>
-      </c>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+    </row>
+    <row r="38" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>188</v>
-      </c>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D40" s="34"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="34"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D42" s="34"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D43" s="34"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D44" s="34"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D45" s="34"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D46" s="34"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D47" s="34"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D48" s="34"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D49" s="34"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="30"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A50" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D50" s="34"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A51" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D51" s="34"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="30"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A52" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D52" s="34"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A53" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D53" s="34"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="30"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A54" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D54" s="34"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D55" s="34"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="30"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A56" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" s="34"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A57" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D57" s="34"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="30"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D58" s="34"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D59" s="34"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="30"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" s="33" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="30"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+    </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
@@ -5203,6 +4087,7 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5226,94 +4111,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="G1" s="28" t="s">
+      <c r="A1" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="H1" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="32">
+      <c r="A2" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="28">
         <v>43894</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
+      <c r="D2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Aurum sw/client visit form (#1190)
* feat: client visit action

* feat: client visit on review
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331DC98-A299-0048-84F0-C30C612473CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A134CAAD-C151-3C41-8B03-42B72B74A7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-5600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhGA2rHGT2d/E/8q1x8a36p9KSGYA=="/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="212">
   <si>
     <t>type</t>
   </si>
@@ -158,9 +158,6 @@
     <t>../inputs/contact/phone</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>NO_LABEL</t>
   </si>
   <si>
@@ -347,24 +344,15 @@
     <t>Private clinic</t>
   </si>
   <si>
-    <t>select_one client_visit</t>
-  </si>
-  <si>
     <t>Which facility?</t>
   </si>
   <si>
-    <t>selected(${client_visit}, 'chaps_mc_clinic')</t>
-  </si>
-  <si>
     <t>client_visit_location</t>
   </si>
   <si>
     <t>Specify</t>
   </si>
   <si>
-    <t>selected(${client_visit}, 'doh') or selected(${client_visit}, 'private_clinic')</t>
-  </si>
-  <si>
     <t>Client reached by phone and is ok</t>
   </si>
   <si>
@@ -393,6 +381,288 @@
   </si>
   <si>
     <t>instance::tag</t>
+  </si>
+  <si>
+    <t>select_one visit</t>
+  </si>
+  <si>
+    <t>select_one districts</t>
+  </si>
+  <si>
+    <t>select_one sites</t>
+  </si>
+  <si>
+    <t>select_one ae_severity</t>
+  </si>
+  <si>
+    <t>visit</t>
+  </si>
+  <si>
+    <t>phone_credit</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>ae_severity</t>
+  </si>
+  <si>
+    <t>ae_code</t>
+  </si>
+  <si>
+    <t>care_provider</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>What type of visit are you reporting?</t>
+  </si>
+  <si>
+    <t>Verify ZAR 100 phone credit given to client</t>
+  </si>
+  <si>
+    <t>Explain why</t>
+  </si>
+  <si>
+    <t>Date of visit</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Did the provider identify an AE?</t>
+  </si>
+  <si>
+    <t>Adverse Event Code and Timing</t>
+  </si>
+  <si>
+    <t>Name of Health Care Provider who reviewed the client</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>selected(${visit}, 'day14')</t>
+  </si>
+  <si>
+    <t>selected(${phone_credit}, 'no')</t>
+  </si>
+  <si>
+    <t>not(${district} = '')</t>
+  </si>
+  <si>
+    <t>selected(${ae_severity}, 'mild') or selected(${ae_severity}, 'moderate') or selected(${ae_severity}, 'severe')</t>
+  </si>
+  <si>
+    <t>regex(., '^(AN|BL|IN|OT|PA|SD|SX|WD|OA)-[A-C]$') or regex(., '^(an|bl|in|ot|pa|sd|sx|wd|oa)-[a-c]$')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter valid AE Code </t>
+  </si>
+  <si>
+    <t>Note that this is the name of the clinician, copied from the paper Client Intake Form, not the name of the study nurse who uses the software</t>
+  </si>
+  <si>
+    <t>instance::db-doc</t>
+  </si>
+  <si>
+    <t>day14</t>
+  </si>
+  <si>
+    <t>Day 14 Post Circumcision</t>
+  </si>
+  <si>
+    <t>day42</t>
+  </si>
+  <si>
+    <t>Day 42 Post Circumcision</t>
+  </si>
+  <si>
+    <t>additional</t>
+  </si>
+  <si>
+    <t>Additional Review</t>
+  </si>
+  <si>
+    <t>districts</t>
+  </si>
+  <si>
+    <t>ekurhuleni</t>
+  </si>
+  <si>
+    <t>Ekurhuleni</t>
+  </si>
+  <si>
+    <t>bojanala</t>
+  </si>
+  <si>
+    <t>Bojanala</t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>winnie_mandela</t>
+  </si>
+  <si>
+    <t>Winnie Mandela Clinic</t>
+  </si>
+  <si>
+    <t>bafokeng</t>
+  </si>
+  <si>
+    <t>Bafokeng Clinic</t>
+  </si>
+  <si>
+    <t>letlhabile</t>
+  </si>
+  <si>
+    <t>Mobile Unit</t>
+  </si>
+  <si>
+    <t>mogwase</t>
+  </si>
+  <si>
+    <t>Mogwase Clinic</t>
+  </si>
+  <si>
+    <t>bapong</t>
+  </si>
+  <si>
+    <t>Bapong Clinic</t>
+  </si>
+  <si>
+    <t>circumcision</t>
+  </si>
+  <si>
+    <t>Circumcision</t>
+  </si>
+  <si>
+    <t>day2</t>
+  </si>
+  <si>
+    <t>Day 2 Post Circumcision</t>
+  </si>
+  <si>
+    <t>day7</t>
+  </si>
+  <si>
+    <t>Day 7 Post Circumcision</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>visit_facility</t>
+  </si>
+  <si>
+    <t>select_one visit_facility</t>
+  </si>
+  <si>
+    <t>selected(${visit_facility}, 'doh') or selected(${visit_facility}, 'private_clinic')</t>
+  </si>
+  <si>
+    <t>selected(${visit_facility}, 'chaps_mc_clinic')</t>
+  </si>
+  <si>
+    <t>instance::db-doc-ref</t>
+  </si>
+  <si>
+    <t>linked_client_visit</t>
+  </si>
+  <si>
+    <t>${client_visit}</t>
+  </si>
+  <si>
+    <t>patient_uuid</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>content_type</t>
+  </si>
+  <si>
+    <t>"xml"</t>
+  </si>
+  <si>
+    <t>"client_visit"</t>
+  </si>
+  <si>
+    <t>"data_record"</t>
+  </si>
+  <si>
+    <t>../../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>${nurse}</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>../../../review/return_client/visit_date</t>
+  </si>
+  <si>
+    <t>client_seen</t>
+  </si>
+  <si>
+    <t>${client_came}</t>
+  </si>
+  <si>
+    <t>facility</t>
+  </si>
+  <si>
+    <t>clinic</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>../../review/return_client/visit_facility</t>
+  </si>
+  <si>
+    <t>../../review/return_client/health_center/name</t>
+  </si>
+  <si>
+    <t>../../review/return_client/client_visit_location</t>
+  </si>
+  <si>
+    <t>../../review/return_client/visit_date</t>
+  </si>
+  <si>
+    <t>../../review/tracing_method</t>
+  </si>
+  <si>
+    <t>../../review/explain</t>
+  </si>
+  <si>
+    <t>../../review/nurse</t>
+  </si>
+  <si>
+    <t>tracing_medium</t>
+  </si>
+  <si>
+    <t>service_provider</t>
   </si>
 </sst>
 </file>
@@ -402,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -505,8 +775,31 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +810,48 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2E75B6"/>
         <bgColor rgb="FF2E75B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -554,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -590,21 +925,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,10 +941,61 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,11 +1211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD15"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -852,12 +1226,14 @@
     <col min="4" max="4" width="37.1640625" customWidth="1"/>
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="52.33203125" customWidth="1"/>
+    <col min="7" max="7" width="44.83203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
     <col min="9" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="25.83203125" customWidth="1"/>
     <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="13" max="26" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16">
@@ -894,11 +1270,15 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="L1" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>182</v>
+      </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -1069,7 +1449,9 @@
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="C9" s="9"/>
       <c r="D9" s="1"/>
       <c r="E9" s="10"/>
@@ -1081,13 +1463,11 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1096,15 +1476,13 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="16">
-      <c r="A11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1112,74 +1490,30 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="16">
-      <c r="A12" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="16">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1189,189 +1523,187 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+    </row>
+    <row r="14" spans="1:26" ht="16">
+      <c r="A14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+    </row>
+    <row r="15" spans="1:26" ht="16">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="13" t="s">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" ht="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" ht="16">
+      <c r="A17" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="B17" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" ht="16">
+      <c r="A18" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-    </row>
-    <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="8" t="s">
+      <c r="B18" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
+      <c r="C18" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-    </row>
-    <row r="16" spans="1:26" ht="16">
-      <c r="A16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-    </row>
-    <row r="17" spans="1:26" ht="16">
-      <c r="A17" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-    </row>
-    <row r="18" spans="1:26" ht="16">
-      <c r="A18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -1386,32 +1718,28 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="16">
-      <c r="A19" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
+      <c r="A19" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
@@ -1426,26 +1754,26 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="16">
-      <c r="A20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
+      <c r="A20" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -1460,22 +1788,26 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="16">
-      <c r="A21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
+      <c r="A21" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="60"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
@@ -1490,28 +1822,34 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="16">
-      <c r="A22" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="A22" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -1526,32 +1864,26 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="16">
-      <c r="A23" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
+      <c r="A23" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="58"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -1566,22 +1898,22 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="16">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -1596,30 +1928,28 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="16">
-      <c r="A25" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="A25" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
@@ -1633,31 +1963,33 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
+    <row r="26" spans="1:26" ht="16">
+      <c r="A26" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
+      <c r="G26" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
@@ -1671,33 +2003,23 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
+    <row r="27" spans="1:26" ht="16">
+      <c r="A27" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="50"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -1711,73 +2033,962 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:26" ht="16">
+      <c r="A28" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="58"/>
+      <c r="F28" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A29" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A30" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A31" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" s="60"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="L31" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A32" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+      <c r="B32" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A34" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="42"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A36" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="43"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A37" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="41"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A38" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="35"/>
+      <c r="F38" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="41"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A39" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="35"/>
+      <c r="F39" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="41"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A40" s="32"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="41"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A41" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="L41" s="35"/>
+      <c r="M41" s="41"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A42" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="41"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A43" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="E43" s="35"/>
+      <c r="F43" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="41"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A44" s="32"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="41"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A45" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="41"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A46" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="35"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="I46" s="35"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="41"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A47" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="33"/>
+      <c r="K47" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="L47" s="35"/>
+      <c r="M47" s="41"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A48" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="41"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A49" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="41"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A50" s="32"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="41"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A51" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="L51" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="41"/>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A52" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="L52" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="41"/>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A53" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="L53" s="35"/>
+      <c r="M53" s="41"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A54" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="L54" s="35"/>
+      <c r="M54" s="41"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A55" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="L55" s="35"/>
+      <c r="M55" s="41"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A56" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="41"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
+      <c r="M56" s="41"/>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A58" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="47"/>
+      <c r="N58" s="47"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A59" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="L59" s="47"/>
+      <c r="M59" s="47"/>
+      <c r="N59" s="47"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A60" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="47"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A61" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="L61" s="47"/>
+      <c r="M61" s="47"/>
+      <c r="N61" s="47"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A62" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+      <c r="J62" s="47"/>
+      <c r="K62" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="L62" s="47"/>
+      <c r="M62" s="47"/>
+      <c r="N62" s="47"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A63" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="L63" s="47"/>
+      <c r="M63" s="47"/>
+      <c r="N63" s="47"/>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A64" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="47"/>
+      <c r="K64" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="L64" s="47"/>
+      <c r="M64" s="47"/>
+      <c r="N64" s="47"/>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A65" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
+      <c r="K65" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="L65" s="47"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="47"/>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A66" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="47"/>
+      <c r="J66" s="47"/>
+      <c r="K66" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="L66" s="47"/>
+      <c r="M66" s="47"/>
+      <c r="N66" s="47"/>
+    </row>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A67" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="B67" s="45"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="47"/>
+      <c r="M67" s="47"/>
+      <c r="N67" s="47"/>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A68" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="47"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="47"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="47"/>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -2700,6 +3911,22 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -2708,11 +3935,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -2724,9 +3951,9 @@
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2734,428 +3961,551 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16">
+      <c r="D1" s="40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16">
-      <c r="A3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16">
+    </row>
+    <row r="4" spans="1:4" ht="16">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" ht="16">
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="16">
-      <c r="A7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16">
-      <c r="A8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16">
+    </row>
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="16">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16">
-      <c r="A11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    <row r="13" spans="1:4" ht="15" customHeight="1">
+      <c r="A13" s="12" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C19" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-    </row>
-    <row r="30" spans="1:3" ht="16">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-    </row>
-    <row r="31" spans="1:3" ht="16">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="39"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="39"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A29" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="39"/>
+    </row>
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="39"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-    </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+      <c r="A35" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="39"/>
+    </row>
+    <row r="36" spans="1:26" s="26" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="39"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="25"/>
+      <c r="X36" s="25"/>
+      <c r="Y36" s="25"/>
+      <c r="Z36" s="25"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-    </row>
-    <row r="38" spans="1:26" s="30" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="29"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A38" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
+      <c r="A39" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
+      <c r="A40" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="30"/>
+      <c r="A41" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="30"/>
+      <c r="A42" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="30"/>
+      <c r="D43" s="26"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="30"/>
+      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="30"/>
+      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="30"/>
+      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="30"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="30"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="30"/>
+      <c r="D49" s="26"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="30"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="30"/>
+      <c r="D51" s="26"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="30"/>
+      <c r="D52" s="26"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="30"/>
+      <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="30"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="30"/>
+      <c r="D55" s="26"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="30"/>
+      <c r="D56" s="26"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="30"/>
+      <c r="D57" s="26"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="30"/>
+      <c r="D58" s="26"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="30"/>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="30"/>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-    </row>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
@@ -4086,8 +5436,6 @@
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -4111,94 +5459,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="24">
+        <v>43894</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="28">
-        <v>43894</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: client visit reports
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A134CAAD-C151-3C41-8B03-42B72B74A7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B124579-90BE-064E-8FBE-61D516486B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-5600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
   <si>
     <t>type</t>
   </si>
@@ -383,33 +383,15 @@
     <t>instance::tag</t>
   </si>
   <si>
-    <t>select_one visit</t>
-  </si>
-  <si>
-    <t>select_one districts</t>
-  </si>
-  <si>
-    <t>select_one sites</t>
-  </si>
-  <si>
     <t>select_one ae_severity</t>
   </si>
   <si>
     <t>visit</t>
   </si>
   <si>
-    <t>phone_credit</t>
-  </si>
-  <si>
-    <t>explanation</t>
-  </si>
-  <si>
     <t>district</t>
   </si>
   <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>ae_severity</t>
   </si>
   <si>
@@ -422,24 +404,12 @@
     <t>comments</t>
   </si>
   <si>
-    <t>What type of visit are you reporting?</t>
-  </si>
-  <si>
-    <t>Verify ZAR 100 phone credit given to client</t>
-  </si>
-  <si>
-    <t>Explain why</t>
-  </si>
-  <si>
     <t>Date of visit</t>
   </si>
   <si>
     <t>District</t>
   </si>
   <si>
-    <t>Site</t>
-  </si>
-  <si>
     <t>Did the provider identify an AE?</t>
   </si>
   <si>
@@ -452,15 +422,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>selected(${visit}, 'day14')</t>
-  </si>
-  <si>
-    <t>selected(${phone_credit}, 'no')</t>
-  </si>
-  <si>
-    <t>not(${district} = '')</t>
-  </si>
-  <si>
     <t>selected(${ae_severity}, 'mild') or selected(${ae_severity}, 'moderate') or selected(${ae_severity}, 'severe')</t>
   </si>
   <si>
@@ -663,6 +624,15 @@
   </si>
   <si>
     <t>service_provider</t>
+  </si>
+  <si>
+    <t>db:district_hospital</t>
+  </si>
+  <si>
+    <t>enrollment_facility</t>
+  </si>
+  <si>
+    <t>VMMC enrollment facility</t>
   </si>
 </sst>
 </file>
@@ -672,7 +642,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -798,6 +768,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -855,7 +850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -885,11 +880,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -995,6 +1005,27 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1211,11 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1013"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1274,10 +1305,10 @@
         <v>117</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1650,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C17" s="55"/>
       <c r="D17" s="56"/>
@@ -1755,10 +1786,10 @@
     </row>
     <row r="20" spans="1:26" ht="16">
       <c r="A20" s="51" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C20" s="59" t="s">
         <v>105</v>
@@ -1832,7 +1863,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="E22" s="58" t="s">
         <v>28</v>
@@ -1938,7 +1969,7 @@
         <v>107</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E25" s="58"/>
       <c r="F25" s="58"/>
@@ -2154,7 +2185,7 @@
         <v>35</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C31" s="60"/>
       <c r="D31" s="58"/>
@@ -2165,14 +2196,14 @@
       <c r="I31" s="58"/>
       <c r="J31" s="58"/>
       <c r="K31" s="58" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="L31" s="58" t="s">
         <v>19</v>
       </c>
       <c r="M31" s="58"/>
       <c r="N31" s="58" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
@@ -2251,7 +2282,7 @@
       <c r="K34" s="41"/>
       <c r="L34" s="41"/>
       <c r="M34" s="43" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
@@ -2274,13 +2305,15 @@
         <v>11</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C36" s="42" t="s">
         <v>43</v>
       </c>
       <c r="D36" s="41"/>
-      <c r="E36" s="42"/>
+      <c r="E36" s="42" t="s">
+        <v>15</v>
+      </c>
       <c r="F36" s="41"/>
       <c r="G36" s="41"/>
       <c r="H36" s="41"/>
@@ -2291,21 +2324,13 @@
       <c r="M36" s="43"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>131</v>
-      </c>
+      <c r="A37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="35"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="36"/>
       <c r="H37" s="35"/>
       <c r="I37" s="35"/>
       <c r="J37" s="33"/>
@@ -2315,247 +2340,233 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
       <c r="A38" s="32" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>141</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D38" s="35"/>
       <c r="E38" s="35"/>
       <c r="F38" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
       <c r="I38" s="35"/>
       <c r="J38" s="33"/>
-      <c r="K38" s="35"/>
+      <c r="K38" s="35" t="s">
+        <v>183</v>
+      </c>
       <c r="L38" s="35"/>
       <c r="M38" s="41"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>124</v>
+      <c r="A39" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>120</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="35"/>
+        <v>126</v>
+      </c>
+      <c r="D39" s="35"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="33" t="s">
         <v>29</v>
       </c>
       <c r="G39" s="36"/>
-      <c r="H39" s="35"/>
+      <c r="H39" s="36"/>
       <c r="I39" s="35"/>
       <c r="J39" s="33"/>
       <c r="K39" s="35"/>
       <c r="L39" s="35"/>
-      <c r="M39" s="41"/>
+      <c r="M39" s="35"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="32"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="E40" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="F40" s="33"/>
       <c r="G40" s="36"/>
-      <c r="H40" s="35"/>
+      <c r="H40" s="36"/>
       <c r="I40" s="35"/>
       <c r="J40" s="33"/>
       <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="41"/>
+      <c r="L40" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M40" s="35"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>52</v>
+      <c r="A41" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>1</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="E41" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="33"/>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
       <c r="I41" s="35"/>
       <c r="J41" s="33"/>
-      <c r="K41" s="35" t="s">
-        <v>196</v>
-      </c>
+      <c r="K41" s="35"/>
       <c r="L41" s="35"/>
-      <c r="M41" s="41"/>
+      <c r="M41" s="35"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>125</v>
-      </c>
+      <c r="A42" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="33"/>
       <c r="C42" s="35" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
       <c r="G42" s="36"/>
       <c r="H42" s="36"/>
       <c r="I42" s="35"/>
       <c r="J42" s="33"/>
       <c r="K42" s="35"/>
       <c r="L42" s="35"/>
-      <c r="M42" s="41"/>
+      <c r="M42" s="35"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
       <c r="G43" s="36"/>
       <c r="H43" s="36"/>
       <c r="I43" s="35"/>
       <c r="J43" s="33"/>
       <c r="K43" s="35"/>
       <c r="L43" s="35"/>
-      <c r="M43" s="41"/>
+      <c r="M43" s="35"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="32"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="33"/>
+      <c r="A44" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69" t="s">
+        <v>29</v>
+      </c>
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
       <c r="I44" s="35"/>
       <c r="J44" s="33"/>
       <c r="K44" s="35"/>
       <c r="L44" s="35"/>
-      <c r="M44" s="41"/>
+      <c r="M44" s="35"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="33" t="s">
-        <v>29</v>
-      </c>
+      <c r="A45" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="71"/>
       <c r="G45" s="36"/>
       <c r="H45" s="36"/>
       <c r="I45" s="35"/>
       <c r="J45" s="33"/>
       <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="41"/>
+      <c r="L45" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="35"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="H46" s="36" t="s">
-        <v>146</v>
-      </c>
+      <c r="B46" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="72"/>
+      <c r="E46" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="69"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="35"/>
       <c r="J46" s="33"/>
       <c r="K46" s="35"/>
       <c r="L46" s="35"/>
-      <c r="M46" s="41"/>
+      <c r="M46" s="35"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35" t="s">
-        <v>147</v>
-      </c>
+      <c r="A47" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="67"/>
+      <c r="C47" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="35"/>
       <c r="J47" s="33"/>
-      <c r="K47" s="35" t="s">
-        <v>193</v>
-      </c>
+      <c r="K47" s="35"/>
       <c r="L47" s="35"/>
-      <c r="M47" s="41"/>
+      <c r="M47" s="35"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>140</v>
-      </c>
+      <c r="A48" s="32"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="35"/>
       <c r="E48" s="35"/>
       <c r="F48" s="33"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="35"/>
       <c r="J48" s="33"/>
       <c r="K48" s="35"/>
@@ -2564,17 +2575,21 @@
     </row>
     <row r="49" spans="1:14" ht="15.75" customHeight="1">
       <c r="A49" s="32" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="35"/>
+        <v>121</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="D49" s="35"/>
       <c r="E49" s="35"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
+      <c r="F49" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
       <c r="I49" s="35"/>
       <c r="J49" s="33"/>
       <c r="K49" s="35"/>
@@ -2582,14 +2597,26 @@
       <c r="M49" s="41"/>
     </row>
     <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="32"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
+      <c r="A50" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="E50" s="35"/>
       <c r="F50" s="33"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
+      <c r="G50" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H50" s="36" t="s">
+        <v>133</v>
+      </c>
       <c r="I50" s="35"/>
       <c r="J50" s="33"/>
       <c r="K50" s="35"/>
@@ -2601,35 +2628,35 @@
         <v>35</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>185</v>
+        <v>123</v>
       </c>
       <c r="C51" s="35" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="D51" s="35"/>
       <c r="E51" s="35"/>
       <c r="F51" s="33"/>
       <c r="G51" s="35"/>
       <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
+      <c r="I51" s="35" t="s">
+        <v>134</v>
+      </c>
       <c r="J51" s="33"/>
       <c r="K51" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="L51" s="35" t="s">
-        <v>19</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="L51" s="35"/>
       <c r="M51" s="41"/>
     </row>
     <row r="52" spans="1:14" ht="15.75" customHeight="1">
       <c r="A52" s="32" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="D52" s="35"/>
       <c r="E52" s="35"/>
@@ -2638,20 +2665,16 @@
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
       <c r="J52" s="33"/>
-      <c r="K52" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="L52" s="35" t="s">
-        <v>19</v>
-      </c>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
       <c r="M52" s="41"/>
     </row>
     <row r="53" spans="1:14" ht="15.75" customHeight="1">
       <c r="A53" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="C53" s="35"/>
       <c r="D53" s="35"/>
@@ -2661,19 +2684,14 @@
       <c r="H53" s="35"/>
       <c r="I53" s="35"/>
       <c r="J53" s="33"/>
-      <c r="K53" s="35" t="s">
-        <v>190</v>
-      </c>
+      <c r="K53" s="35"/>
       <c r="L53" s="35"/>
       <c r="M53" s="41"/>
+      <c r="N53" s="47"/>
     </row>
     <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="34" t="s">
-        <v>177</v>
-      </c>
+      <c r="A54" s="32"/>
+      <c r="B54" s="34"/>
       <c r="C54" s="35"/>
       <c r="D54" s="35"/>
       <c r="E54" s="35"/>
@@ -2682,18 +2700,17 @@
       <c r="H54" s="35"/>
       <c r="I54" s="35"/>
       <c r="J54" s="33"/>
-      <c r="K54" s="35" t="s">
-        <v>189</v>
-      </c>
+      <c r="K54" s="35"/>
       <c r="L54" s="35"/>
       <c r="M54" s="41"/>
+      <c r="N54" s="47"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" customHeight="1">
       <c r="A55" s="32" t="s">
         <v>35</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C55" s="35" t="s">
         <v>43</v>
@@ -2706,141 +2723,147 @@
       <c r="I55" s="35"/>
       <c r="J55" s="33"/>
       <c r="K55" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="L55" s="35"/>
+        <v>178</v>
+      </c>
+      <c r="L55" s="35" t="s">
+        <v>19</v>
+      </c>
       <c r="M55" s="41"/>
+      <c r="N55" s="47"/>
     </row>
     <row r="56" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="L56" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="41"/>
+      <c r="N56" s="47"/>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A57" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="L57" s="35"/>
+      <c r="M57" s="41"/>
+      <c r="N57" s="47"/>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A58" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="L58" s="35"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="47"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A59" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="L59" s="35"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="47"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A60" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B60" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="41"/>
-      <c r="L56" s="41"/>
-      <c r="M56" s="41"/>
-    </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A58" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="47"/>
-      <c r="M58" s="47"/>
-      <c r="N58" s="47"/>
-    </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A59" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="L59" s="47"/>
-      <c r="M59" s="47"/>
-      <c r="N59" s="47"/>
-    </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A60" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="L60" s="47"/>
-      <c r="M60" s="47"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="41"/>
+      <c r="L60" s="41"/>
+      <c r="M60" s="41"/>
       <c r="N60" s="47"/>
     </row>
     <row r="61" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A61" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="48" t="s">
-        <v>204</v>
-      </c>
-      <c r="L61" s="47"/>
-      <c r="M61" s="47"/>
       <c r="N61" s="47"/>
     </row>
     <row r="62" spans="1:14" ht="15.75" customHeight="1">
       <c r="A62" s="46" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C62" s="47"/>
-      <c r="D62" s="47" t="s">
-        <v>180</v>
-      </c>
+      <c r="D62" s="47"/>
       <c r="E62" s="47"/>
       <c r="F62" s="47"/>
       <c r="G62" s="47"/>
       <c r="H62" s="47"/>
       <c r="I62" s="47"/>
       <c r="J62" s="47"/>
-      <c r="K62" s="48" t="s">
-        <v>205</v>
-      </c>
+      <c r="K62" s="47"/>
       <c r="L62" s="47"/>
       <c r="M62" s="47"/>
       <c r="N62" s="47"/>
@@ -2850,12 +2873,10 @@
         <v>35</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="C63" s="47"/>
-      <c r="D63" s="47" t="s">
-        <v>47</v>
-      </c>
+      <c r="D63" s="47"/>
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47"/>
@@ -2863,7 +2884,7 @@
       <c r="I63" s="47"/>
       <c r="J63" s="47"/>
       <c r="K63" s="48" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="L63" s="47"/>
       <c r="M63" s="47"/>
@@ -2874,11 +2895,11 @@
         <v>35</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="C64" s="47"/>
       <c r="D64" s="47" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E64" s="47"/>
       <c r="F64" s="47"/>
@@ -2887,22 +2908,21 @@
       <c r="I64" s="47"/>
       <c r="J64" s="47"/>
       <c r="K64" s="48" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="L64" s="47"/>
       <c r="M64" s="47"/>
-      <c r="N64" s="47"/>
-    </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1">
+    </row>
+    <row r="65" spans="1:13" ht="15.75" customHeight="1">
       <c r="A65" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="C65" s="47"/>
       <c r="D65" s="47" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="E65" s="47"/>
       <c r="F65" s="47"/>
@@ -2911,21 +2931,22 @@
       <c r="I65" s="47"/>
       <c r="J65" s="47"/>
       <c r="K65" s="48" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="L65" s="47"/>
       <c r="M65" s="47"/>
-      <c r="N65" s="47"/>
-    </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1">
+    </row>
+    <row r="66" spans="1:13" ht="15.75" customHeight="1">
       <c r="A66" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
+      <c r="D66" s="47" t="s">
+        <v>167</v>
+      </c>
       <c r="E66" s="47"/>
       <c r="F66" s="47"/>
       <c r="G66" s="47"/>
@@ -2933,62 +2954,145 @@
       <c r="I66" s="47"/>
       <c r="J66" s="47"/>
       <c r="K66" s="48" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="L66" s="47"/>
       <c r="M66" s="47"/>
-      <c r="N66" s="47"/>
-    </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1">
+    </row>
+    <row r="67" spans="1:13" ht="15.75" customHeight="1">
       <c r="A67" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="B67" s="45"/>
+        <v>35</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>52</v>
+      </c>
       <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
+      <c r="D67" s="47" t="s">
+        <v>47</v>
+      </c>
       <c r="E67" s="47"/>
       <c r="F67" s="47"/>
       <c r="G67" s="47"/>
       <c r="H67" s="47"/>
       <c r="I67" s="47"/>
       <c r="J67" s="47"/>
-      <c r="K67" s="47"/>
+      <c r="K67" s="48" t="s">
+        <v>193</v>
+      </c>
       <c r="L67" s="47"/>
       <c r="M67" s="47"/>
-      <c r="N67" s="47"/>
-    </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1">
+    </row>
+    <row r="68" spans="1:13" ht="15.75" customHeight="1">
       <c r="A68" s="46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
+      <c r="D68" s="47" t="s">
+        <v>56</v>
+      </c>
       <c r="E68" s="47"/>
       <c r="F68" s="47"/>
       <c r="G68" s="47"/>
       <c r="H68" s="47"/>
       <c r="I68" s="47"/>
       <c r="J68" s="47"/>
-      <c r="K68" s="47"/>
+      <c r="K68" s="48" t="s">
+        <v>194</v>
+      </c>
       <c r="L68" s="47"/>
       <c r="M68" s="47"/>
-      <c r="N68" s="47"/>
-    </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1"/>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="69" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A69" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
+      <c r="K69" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="L69" s="47"/>
+      <c r="M69" s="47"/>
+    </row>
+    <row r="70" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A70" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
+      <c r="K70" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+    </row>
+    <row r="71" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A71" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71" s="45"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="47"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="47"/>
+      <c r="M71" s="47"/>
+    </row>
+    <row r="72" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A72" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="47"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="47"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
+      <c r="K72" s="47"/>
+      <c r="L72" s="47"/>
+      <c r="M72" s="47"/>
+    </row>
+    <row r="73" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="74" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="75" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="76" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -3922,11 +4026,6 @@
     <row r="1011" ht="15.75" customHeight="1"/>
     <row r="1012" ht="15.75" customHeight="1"/>
     <row r="1013" ht="15.75" customHeight="1"/>
-    <row r="1014" ht="15.75" customHeight="1"/>
-    <row r="1015" ht="15.75" customHeight="1"/>
-    <row r="1016" ht="15.75" customHeight="1"/>
-    <row r="1017" ht="15.75" customHeight="1"/>
-    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -3962,7 +4061,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
@@ -4108,7 +4207,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>99</v>
@@ -4119,7 +4218,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>100</v>
@@ -4130,7 +4229,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>102</v>
@@ -4146,73 +4245,73 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D23" s="39"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D25" s="39"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" s="38" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D27" s="39"/>
     </row>
@@ -4224,7 +4323,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
       <c r="A29" s="38" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>61</v>
@@ -4236,7 +4335,7 @@
     </row>
     <row r="30" spans="1:4" ht="16">
       <c r="A30" s="38" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>71</v>
@@ -4248,7 +4347,7 @@
     </row>
     <row r="31" spans="1:4" ht="16">
       <c r="A31" s="38" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>73</v>
@@ -4260,7 +4359,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
       <c r="A32" s="38" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>75</v>
@@ -4284,25 +4383,25 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="39" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D35" s="39"/>
     </row>
     <row r="36" spans="1:26" s="26" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="39" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D36" s="39"/>
       <c r="E36" s="25"/>
@@ -4335,72 +4434,72 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
fix: client review facilities
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B124579-90BE-064E-8FBE-61D516486B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D59E77-19BC-5F4D-A664-66C78C4E58E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhGA2rHGT2d/E/8q1x8a36p9KSGYA=="/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="199">
   <si>
     <t>type</t>
   </si>
@@ -326,24 +326,6 @@
     <t>client_visit</t>
   </si>
   <si>
-    <t>chaps_mc_clinic</t>
-  </si>
-  <si>
-    <t>doh</t>
-  </si>
-  <si>
-    <t>DOH</t>
-  </si>
-  <si>
-    <t>private_clinic</t>
-  </si>
-  <si>
-    <t>CHAPS MC team</t>
-  </si>
-  <si>
-    <t>Private clinic</t>
-  </si>
-  <si>
     <t>Which facility?</t>
   </si>
   <si>
@@ -407,9 +389,6 @@
     <t>Date of visit</t>
   </si>
   <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>Did the provider identify an AE?</t>
   </si>
   <si>
@@ -626,13 +605,25 @@
     <t>service_provider</t>
   </si>
   <si>
-    <t>db:district_hospital</t>
-  </si>
-  <si>
-    <t>enrollment_facility</t>
-  </si>
-  <si>
-    <t>VMMC enrollment facility</t>
+    <t>team</t>
+  </si>
+  <si>
+    <t>Dedicated/mobile VMMC team</t>
+  </si>
+  <si>
+    <t>DoH nurse</t>
+  </si>
+  <si>
+    <t>visited_facility</t>
+  </si>
+  <si>
+    <t>selected(${visit_facility}, 'team')</t>
+  </si>
+  <si>
+    <t>selected(${visit_facility}, 'nurse')</t>
+  </si>
+  <si>
+    <t>../../../review/return_client/health_center/name</t>
   </si>
 </sst>
 </file>
@@ -642,7 +633,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -728,12 +719,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -766,31 +751,6 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -850,7 +810,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -880,27 +840,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="57">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -922,11 +867,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -947,40 +891,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -998,34 +935,12 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1242,11 +1157,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1013"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1301,14 +1216,14 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" s="37" t="s">
-        <v>169</v>
+      <c r="L1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>162</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1445,7 +1360,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="1"/>
@@ -1537,7 +1452,7 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="16">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1556,61 +1471,61 @@
       <c r="K13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>40</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="16">
       <c r="A15" s="1" t="s">
@@ -1677,28 +1592,28 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="16">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56" t="s">
+      <c r="B17" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56" t="s">
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1713,28 +1628,28 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="16">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58" t="s">
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -1749,28 +1664,28 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="16">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
@@ -1785,26 +1700,26 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="16">
-      <c r="A20" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
+      <c r="A20" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -1819,26 +1734,26 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="16">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
@@ -1853,34 +1768,34 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="16">
-      <c r="A22" s="52" t="s">
+      <c r="A22" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" s="58" t="s">
+      <c r="D22" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="62" t="s">
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -1895,26 +1810,26 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="16">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="62" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="58"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -1929,22 +1844,22 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="16">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -1959,28 +1874,28 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="16">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="58" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
+      <c r="B25" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
@@ -1995,32 +1910,32 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="16">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58" t="s">
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="64" t="s">
+      <c r="H26" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
@@ -2035,22 +1950,22 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="16">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -2065,30 +1980,30 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="16">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="58"/>
-      <c r="F28" s="64" t="s">
+      <c r="E28" s="50"/>
+      <c r="F28" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
@@ -2103,30 +2018,30 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58" t="s">
+      <c r="B29" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
@@ -2141,32 +2056,32 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58" t="s">
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="61" t="s">
+      <c r="G30" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="61" t="s">
+      <c r="H30" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
@@ -2181,29 +2096,29 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58" t="s">
-        <v>171</v>
-      </c>
-      <c r="L31" s="58" t="s">
+      <c r="B31" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="52"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="L31" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58" t="s">
-        <v>171</v>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50" t="s">
+        <v>164</v>
       </c>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
@@ -2219,17 +2134,17 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="46" t="s">
         <v>90</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2249,7 +2164,7 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2262,829 +2177,677 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A34" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42" t="s">
+      <c r="C34" s="34"/>
+      <c r="D34" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="43" t="s">
+      <c r="E34" s="35"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="36"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A36" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="36"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A37" s="26"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="34"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A38" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="L38" s="29"/>
+      <c r="M38" s="34"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A41" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="L41" s="29"/>
+      <c r="M41" s="34"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A42" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="34"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="29"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="34"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A44" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J44" s="27"/>
+      <c r="K44" s="29" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="43"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="44" t="s">
+      <c r="L44" s="29"/>
+      <c r="M44" s="34"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A45" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="34"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A46" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="40"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A47" s="26"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="34"/>
+      <c r="N47" s="40"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A48" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="L48" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="34"/>
+      <c r="N48" s="40"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A49" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="L49" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="34"/>
+      <c r="N49" s="40"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A50" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="L50" s="29"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="40"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A51" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="L51" s="29"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="40"/>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A52" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="L52" s="29"/>
+      <c r="M52" s="34"/>
+      <c r="N52" s="40"/>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A53" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="40"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N54" s="40"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A55" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B55" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A56" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="L56" s="40"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="40"/>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A57" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="43"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="32"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="41"/>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="32" t="s">
+      <c r="C57" s="40"/>
+      <c r="D57" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="L57" s="40"/>
+      <c r="M57" s="40"/>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A58" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B58" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="L58" s="40"/>
+      <c r="M58" s="40"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A59" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="L59" s="40"/>
+      <c r="M59" s="40"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A60" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="L38" s="35"/>
-      <c r="M38" s="41"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A39" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A40" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" s="33"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A41" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="35"/>
-      <c r="E41" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="33"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A42" s="33" t="s">
+      <c r="C60" s="40"/>
+      <c r="D60" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="40"/>
+      <c r="J60" s="40"/>
+      <c r="K60" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="L60" s="40"/>
+      <c r="M60" s="40"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A61" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="40"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="L61" s="40"/>
+      <c r="M61" s="40"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A62" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="L62" s="40"/>
+      <c r="M62" s="40"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A63" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="40"/>
+      <c r="I63" s="40"/>
+      <c r="J63" s="40"/>
+      <c r="K63" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="L63" s="40"/>
+      <c r="M63" s="40"/>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A64" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" s="38"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+      <c r="I64" s="40"/>
+      <c r="J64" s="40"/>
+      <c r="K64" s="40"/>
+      <c r="L64" s="40"/>
+      <c r="M64" s="40"/>
+    </row>
+    <row r="65" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A65" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A44" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="C44" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="71"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M45" s="35"/>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="72"/>
-      <c r="E46" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="69"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A47" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="35"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A48" s="32"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="41"/>
-    </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A49" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="41"/>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="I50" s="35"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="41"/>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="J51" s="33"/>
-      <c r="K51" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="L51" s="35"/>
-      <c r="M51" s="41"/>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A52" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="C52" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="41"/>
-    </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A53" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="41"/>
-      <c r="N53" s="47"/>
-    </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="32"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="47"/>
-    </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A55" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="L55" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M55" s="41"/>
-      <c r="N55" s="47"/>
-    </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A56" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="L56" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M56" s="41"/>
-      <c r="N56" s="47"/>
-    </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A57" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="L57" s="35"/>
-      <c r="M57" s="41"/>
-      <c r="N57" s="47"/>
-    </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A58" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="L58" s="35"/>
-      <c r="M58" s="41"/>
-      <c r="N58" s="47"/>
-    </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A59" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="35" t="s">
+      <c r="B65" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="L59" s="35"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="47"/>
-    </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A60" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="47"/>
-    </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1">
-      <c r="N61" s="47"/>
-    </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A62" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-      <c r="J62" s="47"/>
-      <c r="K62" s="47"/>
-      <c r="L62" s="47"/>
-      <c r="M62" s="47"/>
-      <c r="N62" s="47"/>
-    </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A63" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B63" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="L63" s="47"/>
-      <c r="M63" s="47"/>
-      <c r="N63" s="47"/>
-    </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A64" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="L64" s="47"/>
-      <c r="M64" s="47"/>
-    </row>
-    <row r="65" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A65" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B65" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="L65" s="47"/>
-      <c r="M65" s="47"/>
-    </row>
-    <row r="66" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A66" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B66" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47"/>
-      <c r="J66" s="47"/>
-      <c r="K66" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="L66" s="47"/>
-      <c r="M66" s="47"/>
-    </row>
-    <row r="67" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A67" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="L67" s="47"/>
-      <c r="M67" s="47"/>
-    </row>
-    <row r="68" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A68" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-      <c r="K68" s="48" t="s">
-        <v>194</v>
-      </c>
-      <c r="L68" s="47"/>
-      <c r="M68" s="47"/>
-    </row>
-    <row r="69" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A69" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="L69" s="47"/>
-      <c r="M69" s="47"/>
-    </row>
-    <row r="70" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A70" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B70" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="L70" s="47"/>
-      <c r="M70" s="47"/>
-    </row>
-    <row r="71" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A71" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="B71" s="45"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="47"/>
-      <c r="L71" s="47"/>
-      <c r="M71" s="47"/>
-    </row>
-    <row r="72" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A72" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="47"/>
-      <c r="J72" s="47"/>
-      <c r="K72" s="47"/>
-      <c r="L72" s="47"/>
-      <c r="M72" s="47"/>
-    </row>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40"/>
+      <c r="L65" s="40"/>
+      <c r="M65" s="40"/>
+    </row>
+    <row r="66" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="67" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="68" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="69" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="70" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="71" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="72" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="73" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="74" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="75" spans="1:13" ht="15.75" customHeight="1"/>
@@ -4019,13 +3782,6 @@
     <row r="1004" ht="15.75" customHeight="1"/>
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
-    <row r="1007" ht="15.75" customHeight="1"/>
-    <row r="1008" ht="15.75" customHeight="1"/>
-    <row r="1009" ht="15.75" customHeight="1"/>
-    <row r="1010" ht="15.75" customHeight="1"/>
-    <row r="1011" ht="15.75" customHeight="1"/>
-    <row r="1012" ht="15.75" customHeight="1"/>
-    <row r="1013" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -4037,8 +3793,8 @@
   <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -4060,8 +3816,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>120</v>
+      <c r="D1" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
@@ -4089,7 +3845,7 @@
     <row r="4" spans="1:4" ht="16">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="19"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="1"/>
@@ -4157,25 +3913,25 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>108</v>
+      <c r="C13" s="15" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>110</v>
+      <c r="B14" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
@@ -4185,19 +3941,19 @@
       <c r="B15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>116</v>
+      <c r="C15" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>112</v>
+      <c r="B16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
@@ -4206,408 +3962,383 @@
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>103</v>
+      <c r="A18" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
+      <c r="A19" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A22" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D22" s="39"/>
+      <c r="A22" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A23" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="39"/>
+      <c r="A23" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A24" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="39"/>
+      <c r="A24" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A25" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="38" t="s">
+      <c r="A25" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="33"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A26" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="33"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A28" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="1:4" ht="16">
+      <c r="A29" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="33"/>
+    </row>
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A31" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="33"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A34" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C34" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A26" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B26" s="38" t="s">
+      <c r="D34" s="33"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A35" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C35" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A27" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="38" t="s">
+      <c r="D35" s="33"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="10"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A38" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="B38" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="39"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A28" s="38"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="39"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A29" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="1:4" ht="16">
-      <c r="A30" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="39"/>
-    </row>
-    <row r="31" spans="1:4" ht="16">
-      <c r="A31" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="39"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A32" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="39"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-    </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="39" t="s">
+      <c r="C38" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="D38" s="33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A39" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C39" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="39"/>
-    </row>
-    <row r="36" spans="1:26" s="26" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" s="39" t="s">
+      <c r="D39" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A40" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C40" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="25"/>
-      <c r="V36" s="25"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-    </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-    </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="39" t="s">
+      <c r="D40" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A41" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="C41" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="D41" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A42" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B39" s="39" t="s">
+      <c r="C42" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B41" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="39" t="s">
-        <v>145</v>
+      <c r="D42" s="33" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="26"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="26"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="26"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="26"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="26"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="26"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
-      <c r="D52" s="26"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="26"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="26"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="26"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="26"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
-      <c r="D58" s="26"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -5558,94 +5289,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="22">
         <v>43894</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix: ae timing and minor enrollment age
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D59E77-19BC-5F4D-A664-66C78C4E58E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E416984-E63D-034A-8F7B-55EA6C58ADA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="200">
   <si>
     <t>type</t>
   </si>
@@ -326,9 +326,6 @@
     <t>client_visit</t>
   </si>
   <si>
-    <t>Which facility?</t>
-  </si>
-  <si>
     <t>client_visit_location</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>selected(${ae_severity}, 'mild') or selected(${ae_severity}, 'moderate') or selected(${ae_severity}, 'severe')</t>
   </si>
   <si>
-    <t>regex(., '^(AN|BL|IN|OT|PA|SD|SX|WD|OA)-[A-C]$') or regex(., '^(an|bl|in|ot|pa|sd|sx|wd|oa)-[a-c]$')</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter valid AE Code </t>
   </si>
   <si>
@@ -624,6 +618,15 @@
   </si>
   <si>
     <t>../../../review/return_client/health_center/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>By whom?</t>
+  </si>
+  <si>
+    <t>Should be one of the following AN|BL|IN|OT|PA|SD|SX|WD|OA followed by - and a letter from A to C</t>
   </si>
 </sst>
 </file>
@@ -1159,9 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1173,8 +1176,9 @@
     <col min="5" max="5" width="26.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="44.83203125" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="10" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="25.83203125" customWidth="1"/>
     <col min="12" max="12" width="14.83203125" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
@@ -1217,13 +1221,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N1" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1596,7 +1600,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
@@ -1701,13 +1705,13 @@
     </row>
     <row r="20" spans="1:26" ht="16">
       <c r="A20" s="44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
@@ -1778,7 +1782,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" s="50" t="s">
         <v>28</v>
@@ -1878,13 +1882,13 @@
         <v>16</v>
       </c>
       <c r="B25" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="49" t="s">
-        <v>101</v>
-      </c>
       <c r="D25" s="50" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
@@ -2022,13 +2026,13 @@
         <v>60</v>
       </c>
       <c r="B29" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="D29" s="50" t="s">
         <v>108</v>
-      </c>
-      <c r="D29" s="50" t="s">
-        <v>109</v>
       </c>
       <c r="E29" s="50"/>
       <c r="F29" s="50" t="s">
@@ -2100,7 +2104,7 @@
         <v>35</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C31" s="52"/>
       <c r="D31" s="50"/>
@@ -2111,14 +2115,14 @@
       <c r="I31" s="50"/>
       <c r="J31" s="50"/>
       <c r="K31" s="50" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L31" s="50" t="s">
         <v>19</v>
       </c>
       <c r="M31" s="50"/>
       <c r="N31" s="50" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
@@ -2197,7 +2201,7 @@
       <c r="K34" s="34"/>
       <c r="L34" s="34"/>
       <c r="M34" s="36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
@@ -2220,7 +2224,7 @@
         <v>11</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C36" s="35" t="s">
         <v>43</v>
@@ -2261,7 +2265,7 @@
         <v>52</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
@@ -2273,7 +2277,7 @@
       <c r="I38" s="29"/>
       <c r="J38" s="27"/>
       <c r="K38" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L38" s="29"/>
       <c r="M38" s="34"/>
@@ -2294,7 +2298,9 @@
       <c r="M39" s="29"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A40" s="27"/>
+      <c r="A40" s="27" t="s">
+        <v>197</v>
+      </c>
       <c r="B40" s="27"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
@@ -2313,7 +2319,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
@@ -2324,20 +2330,20 @@
       <c r="I41" s="29"/>
       <c r="J41" s="27"/>
       <c r="K41" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L41" s="29"/>
       <c r="M41" s="34"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
@@ -2357,23 +2363,23 @@
         <v>16</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="27"/>
-      <c r="G43" s="30" t="s">
-        <v>125</v>
-      </c>
+      <c r="G43" s="30"/>
       <c r="H43" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="I43" s="29"/>
+        <v>124</v>
+      </c>
+      <c r="I43" s="29" t="s">
+        <v>199</v>
+      </c>
       <c r="J43" s="27"/>
       <c r="K43" s="29"/>
       <c r="L43" s="29"/>
@@ -2384,10 +2390,10 @@
         <v>35</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -2395,11 +2401,11 @@
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L44" s="29"/>
       <c r="M44" s="34"/>
@@ -2409,10 +2415,10 @@
         <v>16</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -2430,7 +2436,7 @@
         <v>34</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
@@ -2466,7 +2472,7 @@
         <v>35</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C48" s="29" t="s">
         <v>43</v>
@@ -2479,7 +2485,7 @@
       <c r="I48" s="29"/>
       <c r="J48" s="27"/>
       <c r="K48" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L48" s="29" t="s">
         <v>19</v>
@@ -2505,7 +2511,7 @@
       <c r="I49" s="29"/>
       <c r="J49" s="27"/>
       <c r="K49" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L49" s="29" t="s">
         <v>19</v>
@@ -2529,7 +2535,7 @@
       <c r="I50" s="29"/>
       <c r="J50" s="27"/>
       <c r="K50" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L50" s="29"/>
       <c r="M50" s="34"/>
@@ -2540,7 +2546,7 @@
         <v>35</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
@@ -2551,7 +2557,7 @@
       <c r="I51" s="29"/>
       <c r="J51" s="27"/>
       <c r="K51" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L51" s="29"/>
       <c r="M51" s="34"/>
@@ -2562,7 +2568,7 @@
         <v>35</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>43</v>
@@ -2575,7 +2581,7 @@
       <c r="I52" s="29"/>
       <c r="J52" s="27"/>
       <c r="K52" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L52" s="29"/>
       <c r="M52" s="34"/>
@@ -2609,7 +2615,7 @@
         <v>11</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40"/>
@@ -2629,7 +2635,7 @@
         <v>35</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40"/>
@@ -2640,7 +2646,7 @@
       <c r="I56" s="40"/>
       <c r="J56" s="40"/>
       <c r="K56" s="41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L56" s="40"/>
       <c r="M56" s="40"/>
@@ -2651,7 +2657,7 @@
         <v>35</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40" t="s">
@@ -2664,7 +2670,7 @@
       <c r="I57" s="40"/>
       <c r="J57" s="40"/>
       <c r="K57" s="41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L57" s="40"/>
       <c r="M57" s="40"/>
@@ -2674,11 +2680,11 @@
         <v>35</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
@@ -2687,7 +2693,7 @@
       <c r="I58" s="40"/>
       <c r="J58" s="40"/>
       <c r="K58" s="41" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="L58" s="40"/>
       <c r="M58" s="40"/>
@@ -2697,11 +2703,11 @@
         <v>35</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E59" s="40"/>
       <c r="F59" s="40"/>
@@ -2710,7 +2716,7 @@
       <c r="I59" s="40"/>
       <c r="J59" s="40"/>
       <c r="K59" s="41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L59" s="40"/>
       <c r="M59" s="40"/>
@@ -2733,7 +2739,7 @@
       <c r="I60" s="40"/>
       <c r="J60" s="40"/>
       <c r="K60" s="41" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L60" s="40"/>
       <c r="M60" s="40"/>
@@ -2743,7 +2749,7 @@
         <v>35</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40" t="s">
@@ -2756,7 +2762,7 @@
       <c r="I61" s="40"/>
       <c r="J61" s="40"/>
       <c r="K61" s="41" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L61" s="40"/>
       <c r="M61" s="40"/>
@@ -2766,11 +2772,11 @@
         <v>35</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E62" s="40"/>
       <c r="F62" s="40"/>
@@ -2779,7 +2785,7 @@
       <c r="I62" s="40"/>
       <c r="J62" s="40"/>
       <c r="K62" s="41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L62" s="40"/>
       <c r="M62" s="40"/>
@@ -2789,7 +2795,7 @@
         <v>35</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40"/>
@@ -2800,14 +2806,14 @@
       <c r="I63" s="40"/>
       <c r="J63" s="40"/>
       <c r="K63" s="41" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L63" s="40"/>
       <c r="M63" s="40"/>
     </row>
     <row r="64" spans="1:14" ht="15.75" customHeight="1">
       <c r="A64" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B64" s="38"/>
       <c r="C64" s="40"/>
@@ -2827,7 +2833,7 @@
         <v>34</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C65" s="40"/>
       <c r="D65" s="40"/>
@@ -3817,7 +3823,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
@@ -3920,7 +3926,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -3928,10 +3934,10 @@
         <v>80</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
@@ -3942,7 +3948,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
@@ -3950,10 +3956,10 @@
         <v>80</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
@@ -3963,96 +3969,96 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B19" s="33" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D26" s="33"/>
     </row>
@@ -4064,7 +4070,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="32" t="s">
         <v>61</v>
@@ -4076,7 +4082,7 @@
     </row>
     <row r="29" spans="1:4" ht="16">
       <c r="A29" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>71</v>
@@ -4088,7 +4094,7 @@
     </row>
     <row r="30" spans="1:4" ht="16">
       <c r="A30" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>73</v>
@@ -4100,7 +4106,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>75</v>
@@ -4124,25 +4130,25 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="33" t="s">
         <v>135</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>137</v>
       </c>
       <c r="D34" s="33"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D35" s="33"/>
       <c r="E35" s="10"/>
@@ -4181,72 +4187,72 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>142</v>
-      </c>
       <c r="D38" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D41" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
feat: use comment for for all no visit
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1F6B3-1ABE-4B4D-9E09-3A5E08A432A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40425243-1A6D-E448-8EE7-B89D974D0B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-2900" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -964,7 +964,6 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,8 +1182,8 @@
   <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2088,7 +2087,7 @@
         <v>106</v>
       </c>
       <c r="D30" s="50" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="E30" s="50"/>
       <c r="F30" s="50" t="s">
@@ -2244,7 +2243,7 @@
       <c r="B35" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="57"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="35" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
fix: tracing inperson visit to site
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_review.xlsx
+++ b/config/itech-aurum/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/femioni/medic/config-itech/itech-aurum/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40425243-1A6D-E448-8EE7-B89D974D0B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EFD297-728D-8240-B428-E77CD9E8DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="203">
   <si>
     <t>type</t>
   </si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>Please Explain</t>
-  </si>
-  <si>
-    <t>selected(${tracing_method}, 'unknown')</t>
   </si>
   <si>
     <t>No (Creates TRACE CLIENT task)</t>
@@ -1182,8 +1179,8 @@
   <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1240,13 +1237,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N1" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1619,7 +1616,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
@@ -1652,17 +1649,17 @@
     </row>
     <row r="18" spans="1:26" ht="185" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="B18" s="42" t="s">
-        <v>201</v>
-      </c>
       <c r="C18" s="47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F18" s="48"/>
       <c r="G18" s="48"/>
@@ -1760,13 +1757,13 @@
     </row>
     <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
@@ -1837,7 +1834,7 @@
         <v>48</v>
       </c>
       <c r="D23" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="50" t="s">
         <v>28</v>
@@ -1943,7 +1940,7 @@
         <v>99</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
@@ -2159,7 +2156,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" s="52"/>
       <c r="D32" s="50"/>
@@ -2170,14 +2167,14 @@
       <c r="I32" s="50"/>
       <c r="J32" s="50"/>
       <c r="K32" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L32" s="50" t="s">
         <v>19</v>
       </c>
       <c r="M32" s="50"/>
       <c r="N32" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
@@ -2256,7 +2253,7 @@
       <c r="K35" s="34"/>
       <c r="L35" s="34"/>
       <c r="M35" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2279,7 +2276,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="35" t="s">
         <v>43</v>
@@ -2320,7 +2317,7 @@
         <v>52</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
@@ -2332,7 +2329,7 @@
       <c r="I39" s="29"/>
       <c r="J39" s="27"/>
       <c r="K39" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L39" s="29"/>
       <c r="M39" s="34"/>
@@ -2354,7 +2351,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B41" s="27"/>
       <c r="C41" s="29"/>
@@ -2374,7 +2371,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
@@ -2385,20 +2382,20 @@
       <c r="I42" s="29"/>
       <c r="J42" s="27"/>
       <c r="K42" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L42" s="29"/>
       <c r="M42" s="34"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
@@ -2418,22 +2415,22 @@
         <v>16</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="27"/>
       <c r="G44" s="30"/>
       <c r="H44" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="29"/>
@@ -2445,10 +2442,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -2456,11 +2453,11 @@
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L45" s="29"/>
       <c r="M45" s="34"/>
@@ -2470,10 +2467,10 @@
         <v>16</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
@@ -2491,7 +2488,7 @@
         <v>34</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
@@ -2527,7 +2524,7 @@
         <v>35</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C49" s="29" t="s">
         <v>43</v>
@@ -2540,7 +2537,7 @@
       <c r="I49" s="29"/>
       <c r="J49" s="27"/>
       <c r="K49" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L49" s="29" t="s">
         <v>19</v>
@@ -2566,7 +2563,7 @@
       <c r="I50" s="29"/>
       <c r="J50" s="27"/>
       <c r="K50" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L50" s="29" t="s">
         <v>19</v>
@@ -2590,7 +2587,7 @@
       <c r="I51" s="29"/>
       <c r="J51" s="27"/>
       <c r="K51" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L51" s="29"/>
       <c r="M51" s="34"/>
@@ -2601,7 +2598,7 @@
         <v>35</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
@@ -2612,7 +2609,7 @@
       <c r="I52" s="29"/>
       <c r="J52" s="27"/>
       <c r="K52" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L52" s="29"/>
       <c r="M52" s="34"/>
@@ -2623,7 +2620,7 @@
         <v>35</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="29" t="s">
         <v>43</v>
@@ -2636,7 +2633,7 @@
       <c r="I53" s="29"/>
       <c r="J53" s="27"/>
       <c r="K53" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L53" s="29"/>
       <c r="M53" s="34"/>
@@ -2670,7 +2667,7 @@
         <v>11</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40"/>
@@ -2690,7 +2687,7 @@
         <v>35</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40"/>
@@ -2701,7 +2698,7 @@
       <c r="I57" s="40"/>
       <c r="J57" s="40"/>
       <c r="K57" s="41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L57" s="40"/>
       <c r="M57" s="40"/>
@@ -2712,7 +2709,7 @@
         <v>35</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40" t="s">
@@ -2725,7 +2722,7 @@
       <c r="I58" s="40"/>
       <c r="J58" s="40"/>
       <c r="K58" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L58" s="40"/>
       <c r="M58" s="40"/>
@@ -2735,11 +2732,11 @@
         <v>35</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E59" s="40"/>
       <c r="F59" s="40"/>
@@ -2748,7 +2745,7 @@
       <c r="I59" s="40"/>
       <c r="J59" s="40"/>
       <c r="K59" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L59" s="40"/>
       <c r="M59" s="40"/>
@@ -2758,11 +2755,11 @@
         <v>35</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="40"/>
@@ -2771,7 +2768,7 @@
       <c r="I60" s="40"/>
       <c r="J60" s="40"/>
       <c r="K60" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L60" s="40"/>
       <c r="M60" s="40"/>
@@ -2794,7 +2791,7 @@
       <c r="I61" s="40"/>
       <c r="J61" s="40"/>
       <c r="K61" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L61" s="40"/>
       <c r="M61" s="40"/>
@@ -2804,10 +2801,10 @@
         <v>35</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C62" s="40"/>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="41" t="s">
         <v>56</v>
       </c>
       <c r="E62" s="40"/>
@@ -2817,7 +2814,7 @@
       <c r="I62" s="40"/>
       <c r="J62" s="40"/>
       <c r="K62" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L62" s="40"/>
       <c r="M62" s="40"/>
@@ -2830,8 +2827,8 @@
         <v>105</v>
       </c>
       <c r="C63" s="40"/>
-      <c r="D63" s="40" t="s">
-        <v>107</v>
+      <c r="D63" s="41" t="s">
+        <v>56</v>
       </c>
       <c r="E63" s="40"/>
       <c r="F63" s="40"/>
@@ -2840,7 +2837,7 @@
       <c r="I63" s="40"/>
       <c r="J63" s="40"/>
       <c r="K63" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L63" s="40"/>
       <c r="M63" s="40"/>
@@ -2850,7 +2847,7 @@
         <v>35</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
@@ -2861,14 +2858,14 @@
       <c r="I64" s="40"/>
       <c r="J64" s="40"/>
       <c r="K64" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L64" s="40"/>
       <c r="M64" s="40"/>
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B65" s="38"/>
       <c r="C65" s="40"/>
@@ -2888,7 +2885,7 @@
         <v>34</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C66" s="40"/>
       <c r="D66" s="40"/>
@@ -3878,7 +3875,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -4003,7 +4000,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4024,96 +4021,96 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="33" t="s">
         <v>189</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="33" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="32" t="s">
         <v>148</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>149</v>
       </c>
       <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>150</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>151</v>
       </c>
       <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="32" t="s">
         <v>152</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>153</v>
       </c>
       <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="32" t="s">
         <v>126</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>127</v>
       </c>
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B25" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="32" t="s">
         <v>128</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>129</v>
       </c>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>130</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>131</v>
       </c>
       <c r="D26" s="33"/>
     </row>
@@ -4125,7 +4122,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="32" t="s">
         <v>61</v>
@@ -4137,7 +4134,7 @@
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>71</v>
@@ -4149,7 +4146,7 @@
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>73</v>
@@ -4161,7 +4158,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>75</v>
@@ -4185,25 +4182,25 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="C34" s="33" t="s">
         <v>133</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>134</v>
       </c>
       <c r="D34" s="33"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="33" t="s">
         <v>135</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>136</v>
       </c>
       <c r="D35" s="33"/>
       <c r="E35" s="10"/>
@@ -4242,72 +4239,72 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="C38" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="33" t="s">
-        <v>139</v>
-      </c>
       <c r="D38" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="33" t="s">
-        <v>141</v>
-      </c>
       <c r="D39" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="33" t="s">
-        <v>143</v>
-      </c>
       <c r="D40" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="33" t="s">
-        <v>145</v>
-      </c>
       <c r="D41" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="33" t="s">
-        <v>147</v>
-      </c>
       <c r="D42" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5399,7 +5396,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
         <v>89</v>

</xml_diff>